<commit_message>
Added comments and cleaned the output
</commit_message>
<xml_diff>
--- a/Openspace_ordering.xlsx
+++ b/Openspace_ordering.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kevin J</t>
+          <t>Vera</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Boitumelo</t>
+          <t>David</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dhanya</t>
+          <t>An</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Edoardo</t>
+          <t>Kevin J</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Karthika</t>
+          <t>Jessica</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Andrii</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Miriam</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Beatriz</t>
+          <t>Imad</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Patrick</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Andrii</t>
+          <t>Fatemeh</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Maxim</t>
+          <t>Mohamad</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Stef</t>
+          <t>Patrycja</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Therese</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Oscar</t>
+          <t>Miro</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nina</t>
+          <t>Frank</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Manel</t>
+          <t>Olha</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mohamad</t>
+          <t>Beatriz</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Dhanya</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Therese</t>
+          <t>Manel</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Miro</t>
+          <t>Celina</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Miriam</t>
+          <t>Aleksander</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fatemeh</t>
+          <t>Oscar</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Celina</t>
+          <t>Edoardo</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Kevin P</t>
         </is>
       </c>
     </row>

</xml_diff>